<commit_message>
kod böyle yazılır işte
</commit_message>
<xml_diff>
--- a/portfolyo/Calisma2/Calisma2VeriSet/Egitim_Durum_VS.xlsx
+++ b/portfolyo/Calisma2/Calisma2VeriSet/Egitim_Durum_VS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdemirtas\Desktop\İş analitiği ödev 15.05.2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\myalcin\Documents\GitHub\muy665-bahar2024-takim-kodlar-vadisi\portfolyo\Calisma2\Calisma2VeriSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE998083-BECF-4581-8E64-B07CBD9CF187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9FB560B-AC07-41C3-A3B5-EE5275E2DA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{45343556-FCB3-4A8B-9599-EA76EAB69F1F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15750" xr2:uid="{45343556-FCB3-4A8B-9599-EA76EAB69F1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t>Okuma yazma bilen fakat bir okul bitirmeyen</t>
   </si>
   <si>
-    <t>İlkokul</t>
-  </si>
-  <si>
     <t>Ortaokul veya dengi meslek okul</t>
   </si>
   <si>
@@ -68,9 +65,6 @@
     <t>Lise dengi meslek okul</t>
   </si>
   <si>
-    <t>Yüksekokul veya fakülte</t>
-  </si>
-  <si>
     <t>2014 Ocak</t>
   </si>
   <si>
@@ -398,7 +392,13 @@
     <t>2005 Aralık</t>
   </si>
   <si>
-    <t>Açık öğretim</t>
+    <t>Acik Ogretim</t>
+  </si>
+  <si>
+    <t>Yuksekokul veya fakulte</t>
+  </si>
+  <si>
+    <t>Ilkokul</t>
   </si>
 </sst>
 </file>
@@ -983,48 +983,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="%20 - Vurgu1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="%20 - Vurgu2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="%20 - Vurgu3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="%20 - Vurgu4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="%20 - Vurgu5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="%20 - Vurgu6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="%40 - Vurgu1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="%40 - Vurgu2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="%40 - Vurgu3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="%40 - Vurgu4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="%40 - Vurgu5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="%40 - Vurgu6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="%60 - Vurgu1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="%60 - Vurgu2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="%60 - Vurgu3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="%60 - Vurgu4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="%60 - Vurgu5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="%60 - Vurgu6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Açıklama Metni" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Ana Başlık" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Bağlı Hücre" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Başlık 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Başlık 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Başlık 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Başlık 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Çıkış" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Giriş" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Hesaplama" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="İşaretli Hücre" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="İyi" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Kötü" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Not" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Nötr" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Toplam" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Uyarı Metni" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Vurgu1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Vurgu2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Vurgu3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Vurgu4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Vurgu5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Vurgu6" xfId="38" builtinId="49" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1040,7 +1040,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1359,12 +1359,12 @@
   <dimension ref="A1:J119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1378,7 +1378,7 @@
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
@@ -1392,7 +1392,7 @@
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
     </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -1404,18 +1404,18 @@
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:10" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:10" ht="68.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
@@ -1427,7 +1427,7 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:10" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="57" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="5" t="s">
@@ -1437,27 +1437,27 @@
         <v>5</v>
       </c>
       <c r="E10" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="G10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="H10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="I10" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>11</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="7">
@@ -1485,9 +1485,9 @@
         <v>16.2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="7">
@@ -1515,9 +1515,9 @@
         <v>17.3</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="7">
@@ -1545,9 +1545,9 @@
         <v>17.2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="7">
@@ -1575,9 +1575,9 @@
         <v>15.9</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="7">
@@ -1605,9 +1605,9 @@
         <v>14.3</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="7">
@@ -1635,9 +1635,9 @@
         <v>13.1</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="7">
@@ -1665,9 +1665,9 @@
         <v>13.1</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="7">
@@ -1695,9 +1695,9 @@
         <v>13.7</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="7">
@@ -1725,9 +1725,9 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="7">
@@ -1755,9 +1755,9 @@
         <v>14.6</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="7">
@@ -1785,9 +1785,9 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="7">
@@ -1815,9 +1815,9 @@
         <v>15.2</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="7">
@@ -1845,9 +1845,9 @@
         <v>15.3</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="7">
@@ -1875,9 +1875,9 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="7">
@@ -1905,9 +1905,9 @@
         <v>16.100000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="7">
@@ -1935,9 +1935,9 @@
         <v>15.2</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="7">
@@ -1965,9 +1965,9 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="7">
@@ -1995,9 +1995,9 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="7">
@@ -2025,9 +2025,9 @@
         <v>13.1</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="7">
@@ -2055,9 +2055,9 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="7">
@@ -2085,9 +2085,9 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="7">
@@ -2115,9 +2115,9 @@
         <v>12.6</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="7">
@@ -2145,9 +2145,9 @@
         <v>12.7</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="7">
@@ -2175,9 +2175,9 @@
         <v>13.9</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="7">
@@ -2205,9 +2205,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="7">
@@ -2235,9 +2235,9 @@
         <v>18.600000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="7">
@@ -2265,9 +2265,9 @@
         <v>17.399999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="7">
@@ -2295,9 +2295,9 @@
         <v>15.6</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="7">
@@ -2325,9 +2325,9 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="7">
@@ -2355,9 +2355,9 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="7">
@@ -2385,9 +2385,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="7">
@@ -2415,9 +2415,9 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="7">
@@ -2445,9 +2445,9 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="7">
@@ -2475,9 +2475,9 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="7">
@@ -2505,9 +2505,9 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="7">
@@ -2535,9 +2535,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="7">
@@ -2565,9 +2565,9 @@
         <v>15.1</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="7">
@@ -2595,9 +2595,9 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="7">
@@ -2625,9 +2625,9 @@
         <v>22.7</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="7">
@@ -2655,9 +2655,9 @@
         <v>20.9</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="7">
@@ -2685,9 +2685,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="7">
@@ -2715,9 +2715,9 @@
         <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="7">
@@ -2745,9 +2745,9 @@
         <v>16.2</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="7">
@@ -2775,9 +2775,9 @@
         <v>15.9</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="7">
@@ -2805,9 +2805,9 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="7">
@@ -2835,9 +2835,9 @@
         <v>17.399999999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="7">
@@ -2865,9 +2865,9 @@
         <v>17.8</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="7">
@@ -2895,9 +2895,9 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="7">
@@ -2925,9 +2925,9 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="7">
@@ -2955,9 +2955,9 @@
         <v>27.3</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="7">
@@ -2985,9 +2985,9 @@
         <v>26.8</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="7">
@@ -3015,9 +3015,9 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="7">
@@ -3045,9 +3045,9 @@
         <v>23.3</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="7">
@@ -3075,9 +3075,9 @@
         <v>21.9</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B65" s="1"/>
       <c r="C65" s="7">
@@ -3105,9 +3105,9 @@
         <v>20.9</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="7">
@@ -3135,9 +3135,9 @@
         <v>19.7</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="7">
@@ -3165,9 +3165,9 @@
         <v>19.600000000000001</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B68" s="1"/>
       <c r="C68" s="7">
@@ -3195,9 +3195,9 @@
         <v>20.9</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="7">
@@ -3225,9 +3225,9 @@
         <v>20.9</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="7">
@@ -3255,9 +3255,9 @@
         <v>21.4</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B71" s="1"/>
       <c r="C71" s="7">
@@ -3285,9 +3285,9 @@
         <v>21.4</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="7">
@@ -3315,9 +3315,9 @@
         <v>19.600000000000001</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="7">
@@ -3345,9 +3345,9 @@
         <v>18.8</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B74" s="1"/>
       <c r="C74" s="7">
@@ -3375,9 +3375,9 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="7">
@@ -3405,9 +3405,9 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="7">
@@ -3435,9 +3435,9 @@
         <v>13.7</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B77" s="1"/>
       <c r="C77" s="7">
@@ -3465,9 +3465,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B78" s="1"/>
       <c r="C78" s="7">
@@ -3495,9 +3495,9 @@
         <v>15.9</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="7">
@@ -3525,9 +3525,9 @@
         <v>16.100000000000001</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B80" s="1"/>
       <c r="C80" s="7">
@@ -3555,9 +3555,9 @@
         <v>16.8</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B81" s="1"/>
       <c r="C81" s="7">
@@ -3585,9 +3585,9 @@
         <v>18.100000000000001</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B82" s="1"/>
       <c r="C82" s="7">
@@ -3615,9 +3615,9 @@
         <v>21.9</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B83" s="1"/>
       <c r="C83" s="7">
@@ -3645,9 +3645,9 @@
         <v>24.8</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B84" s="1"/>
       <c r="C84" s="7">
@@ -3675,9 +3675,9 @@
         <v>16.100000000000001</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B85" s="1"/>
       <c r="C85" s="7">
@@ -3705,9 +3705,9 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B86" s="1"/>
       <c r="C86" s="7">
@@ -3735,9 +3735,9 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B87" s="1"/>
       <c r="C87" s="7">
@@ -3765,9 +3765,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B88" s="1"/>
       <c r="C88" s="7">
@@ -3795,9 +3795,9 @@
         <v>16.2</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B89" s="1"/>
       <c r="C89" s="7">
@@ -3825,9 +3825,9 @@
         <v>17.2</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B90" s="1"/>
       <c r="C90" s="7">
@@ -3855,9 +3855,9 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B91" s="1"/>
       <c r="C91" s="7">
@@ -3885,9 +3885,9 @@
         <v>16.100000000000001</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B92" s="1"/>
       <c r="C92" s="7">
@@ -3915,9 +3915,9 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B93" s="1"/>
       <c r="C93" s="7">
@@ -3945,9 +3945,9 @@
         <v>14.7</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B94" s="1"/>
       <c r="C94" s="7">
@@ -3975,9 +3975,9 @@
         <v>16.2</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B95" s="1"/>
       <c r="C95" s="7">
@@ -4005,9 +4005,9 @@
         <v>18.2</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B96" s="1"/>
       <c r="C96" s="7">
@@ -4035,9 +4035,9 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B97" s="1"/>
       <c r="C97" s="7">
@@ -4065,9 +4065,9 @@
         <v>18.8</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B98" s="1"/>
       <c r="C98" s="7">
@@ -4095,9 +4095,9 @@
         <v>17.8</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B99" s="1"/>
       <c r="C99" s="7">
@@ -4125,9 +4125,9 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B100" s="1"/>
       <c r="C100" s="7">
@@ -4155,9 +4155,9 @@
         <v>15.2</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B101" s="1"/>
       <c r="C101" s="7">
@@ -4185,9 +4185,9 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B102" s="1"/>
       <c r="C102" s="7">
@@ -4215,9 +4215,9 @@
         <v>15.7</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B103" s="1"/>
       <c r="C103" s="7">
@@ -4245,9 +4245,9 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B104" s="1"/>
       <c r="C104" s="7">
@@ -4275,9 +4275,9 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B105" s="1"/>
       <c r="C105" s="7">
@@ -4305,9 +4305,9 @@
         <v>13.9</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B106" s="1"/>
       <c r="C106" s="7">
@@ -4335,9 +4335,9 @@
         <v>13.4</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B107" s="1"/>
       <c r="C107" s="7">
@@ -4365,9 +4365,9 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B108" s="1"/>
       <c r="C108" s="7">
@@ -4395,9 +4395,9 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B109" s="1"/>
       <c r="C109" s="7">
@@ -4425,9 +4425,9 @@
         <v>15.3</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B110" s="1"/>
       <c r="C110" s="7">
@@ -4455,9 +4455,9 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B111" s="1"/>
       <c r="C111" s="7">
@@ -4485,9 +4485,9 @@
         <v>13.3</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B112" s="1"/>
       <c r="C112" s="7">
@@ -4515,9 +4515,9 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="113" spans="1:10" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A113" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B113" s="1"/>
       <c r="C113" s="7">
@@ -4545,9 +4545,9 @@
         <v>13.1</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B114" s="1"/>
       <c r="C114" s="7">
@@ -4575,9 +4575,9 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A115" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B115" s="1"/>
       <c r="C115" s="7">
@@ -4605,9 +4605,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B116" s="1"/>
       <c r="C116" s="7">
@@ -4635,9 +4635,9 @@
         <v>15.2</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B117" s="1"/>
       <c r="C117" s="7">
@@ -4665,9 +4665,9 @@
         <v>14.9</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B118" s="1"/>
       <c r="C118" s="7">
@@ -4695,9 +4695,9 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B119" s="1"/>
       <c r="C119" s="7">

</xml_diff>